<commit_message>
Updated module 8 techn. review
</commit_message>
<xml_diff>
--- a/exams/information.xlsx
+++ b/exams/information.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yg/code/github/EN.585.607.82.SP22_Molecular_Biology/exams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E83F866-91FB-0843-8EDA-04E82032AB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB28357-8C65-3F45-B6B4-7C6A19A0FE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{0375DEE7-0427-3C4A-ABDA-053CF52F533B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -399,15 +399,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3995167-7399-A045-AEFA-9CD55C144589}">
-  <dimension ref="C6:D12"/>
+  <dimension ref="C6:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>1</v>
       </c>
@@ -415,7 +415,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>0</v>
       </c>
@@ -423,7 +423,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>2</v>
       </c>
@@ -431,16 +431,29 @@
         <f>D7/D6</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <f>D9*G9</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>3</v>
       </c>
       <c r="D11">
         <v>140</v>
       </c>
-    </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <f>G10/D7</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>4</v>
       </c>

</xml_diff>